<commit_message>
Counting how many of the different numbers there are in the dataset, and made a utility to create moving averages plots
</commit_message>
<xml_diff>
--- a/experiments/Template.xlsx
+++ b/experiments/Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="10485" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="10485" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lonely_GA_Acc" sheetId="1" r:id="rId1"/>
@@ -655,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V112"/>
   <sheetViews>
-    <sheetView topLeftCell="E88" workbookViewId="0">
+    <sheetView topLeftCell="B67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S21" sqref="S21:V112"/>
     </sheetView>
   </sheetViews>
@@ -6886,7 +6886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V105"/>
   <sheetViews>
-    <sheetView topLeftCell="I66" workbookViewId="0">
+    <sheetView topLeftCell="B59" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S21" sqref="S21:V105"/>
     </sheetView>
   </sheetViews>
@@ -11455,11 +11455,11 @@
         <v>0.19608357009291599</v>
       </c>
       <c r="S86">
-        <f t="shared" ref="S86:S112" si="3">M86</f>
+        <f t="shared" ref="S86:S105" si="3">M86</f>
         <v>65</v>
       </c>
       <c r="T86">
-        <f t="shared" ref="T86:U112" si="4">AVERAGE(D86,J86,P86)</f>
+        <f t="shared" ref="T86:U105" si="4">AVERAGE(D86,J86,P86)</f>
         <v>0.93733333333333346</v>
       </c>
       <c r="U86">
@@ -11467,7 +11467,7 @@
         <v>0.19523134468992498</v>
       </c>
       <c r="V86">
-        <f t="shared" ref="V86:V112" si="5">AVERAGE(B86,H86,N86)</f>
+        <f t="shared" ref="V86:V105" si="5">AVERAGE(B86,H86,N86)</f>
         <v>1645130</v>
       </c>
     </row>
@@ -12677,8 +12677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView topLeftCell="I19" workbookViewId="0">
-      <selection activeCell="V102" sqref="S21:V102"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17245,11 +17245,11 @@
         <v>0.20376256996393199</v>
       </c>
       <c r="S86">
-        <f t="shared" ref="S86:S112" si="3">M86</f>
+        <f t="shared" ref="S86:S102" si="3">M86</f>
         <v>65</v>
       </c>
       <c r="T86">
-        <f t="shared" ref="T86:U112" si="4">AVERAGE(D86,J86,P86)</f>
+        <f t="shared" ref="T86:U102" si="4">AVERAGE(D86,J86,P86)</f>
         <v>0.93466666666666676</v>
       </c>
       <c r="U86">
@@ -17257,7 +17257,7 @@
         <v>0.20128057172894431</v>
       </c>
       <c r="V86">
-        <f t="shared" ref="V86:V112" si="5">AVERAGE(B86,H86,N86)</f>
+        <f t="shared" ref="V86:V102" si="5">AVERAGE(B86,H86,N86)</f>
         <v>1725955</v>
       </c>
     </row>
@@ -18278,7 +18278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A178" sqref="A178:A262"/>
     </sheetView>
   </sheetViews>

</xml_diff>